<commit_message>
electrochemical sensors test results
</commit_message>
<xml_diff>
--- a/1-SystemDocs/0-Testing/Chamber_measurements.xlsx
+++ b/1-SystemDocs/0-Testing/Chamber_measurements.xlsx
@@ -817,44 +817,6 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>141</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>1067062</xdr:colOff>
-      <xdr:row>155</xdr:row>
-      <xdr:rowOff>43961</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="11" name="Obrázok 10"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8447942" y="26963077"/>
-          <a:ext cx="5345985" cy="2710961"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
       <xdr:row>157</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -872,7 +834,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -889,18 +851,56 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>7327</xdr:colOff>
+      <xdr:row>141</xdr:row>
+      <xdr:rowOff>146539</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1088409</xdr:colOff>
+      <xdr:row>156</xdr:row>
+      <xdr:rowOff>7327</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Obrázok 14"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8455269" y="27109616"/>
+          <a:ext cx="5360005" cy="2718288"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>644769</xdr:colOff>
-      <xdr:row>150</xdr:row>
-      <xdr:rowOff>29308</xdr:rowOff>
+      <xdr:colOff>7327</xdr:colOff>
+      <xdr:row>148</xdr:row>
+      <xdr:rowOff>153866</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>908538</xdr:colOff>
+      <xdr:colOff>871904</xdr:colOff>
       <xdr:row>166</xdr:row>
-      <xdr:rowOff>161192</xdr:rowOff>
+      <xdr:rowOff>183173</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -909,13 +909,13 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10484827" y="28706885"/>
-          <a:ext cx="2073519" cy="3187211"/>
+          <a:off x="9847385" y="28450443"/>
+          <a:ext cx="2674327" cy="3458307"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln w="28575">
           <a:tailEnd type="triangle"/>
         </a:ln>
       </xdr:spPr>
@@ -1204,8 +1204,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C134" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E166" sqref="E166"/>
+    <sheetView tabSelected="1" topLeftCell="C99" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E158" sqref="E158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>